<commit_message>
day 23 - workings xls with part 1 answer
</commit_message>
<xml_diff>
--- a/Day24/workings.xlsx
+++ b/Day24/workings.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tesco-my.sharepoint.com/personal/craig_roberts_tesco_com/Documents/Dev/AdventOfCode/2021/day24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{00D1E0BB-CE7E-0847-B0EE-23108141FACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DA45F4E-E365-D840-96EE-D679D2E92DF3}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{00D1E0BB-CE7E-0847-B0EE-23108141FACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17C00F28-096B-C84A-968A-F79AD817EFB0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" activeTab="1" xr2:uid="{EE91BE35-D1EB-AA47-8F81-87C2CF2B9ACF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" activeTab="2" xr2:uid="{EE91BE35-D1EB-AA47-8F81-87C2CF2B9ACF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -403,20 +404,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -467,6 +456,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1062,44 +1063,44 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="8"/>
-      <c r="AB7" s="8"/>
-      <c r="AC7" s="8" t="s">
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AD7" s="5"/>
+      <c r="AD7" s="3"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
@@ -1156,55 +1157,55 @@
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="22" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="21" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="T11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="V11" s="4" t="s">
+      <c r="V11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="X11" s="4" t="s">
+      <c r="X11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="Z11" s="4" t="s">
+      <c r="Z11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="AB11" s="4" t="s">
+      <c r="AB11" s="21" t="s">
         <v>25</v>
       </c>
       <c r="AC11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AD11" s="4" t="s">
+      <c r="AD11" s="21" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1212,29 +1213,29 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Z12" s="3"/>
-      <c r="AB12" s="3"/>
+      <c r="H12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Z12" s="24"/>
+      <c r="AB12" s="24"/>
       <c r="AC12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AD12" s="4"/>
+      <c r="AD12" s="21"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
@@ -1338,7 +1339,7 @@
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="23" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -1355,7 +1356,7 @@
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1370,7 +1371,7 @@
       <c r="C19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1468,884 +1469,896 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F45F3D9-96BF-4043-A1CB-C8CA72791154}">
   <dimension ref="A2:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="9"/>
-    <col min="2" max="2" width="17.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11">
+    <row r="2" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7">
         <v>0</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="7">
         <v>2</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="7">
         <v>3</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="7">
         <v>4</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="7">
         <v>5</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="7">
         <v>6</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="7">
         <v>7</v>
       </c>
-      <c r="J2" s="11">
-        <v>8</v>
-      </c>
-      <c r="K2" s="11">
-        <v>9</v>
-      </c>
-      <c r="L2" s="11">
-        <v>10</v>
-      </c>
-      <c r="M2" s="11">
+      <c r="J2" s="7">
+        <v>8</v>
+      </c>
+      <c r="K2" s="7">
+        <v>9</v>
+      </c>
+      <c r="L2" s="7">
+        <v>10</v>
+      </c>
+      <c r="M2" s="7">
         <v>11</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="7">
         <v>12</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="7">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="13" t="s">
+      <c r="N4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="M5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="M6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="N6" s="16" t="s">
+      <c r="N6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O6" s="17" t="s">
+      <c r="O6" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="N7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="13" t="s">
+      <c r="N8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="M9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="13" t="s">
+      <c r="N9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="O9" s="14" t="s">
+      <c r="O9" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="K10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="L10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="N10" s="16" t="s">
+      <c r="N10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="17" t="s">
+      <c r="O10" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="19" t="s">
+      <c r="N11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="O11" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="N12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="O12" s="17" t="s">
+      <c r="B12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="O13" s="17" t="s">
+      <c r="B13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O13" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="N14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="O14" s="17" t="s">
+      <c r="B14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="19" t="s">
+      <c r="L15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="19" t="s">
+      <c r="M15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N15" s="19" t="s">
+      <c r="N15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="O15" s="20" t="s">
+      <c r="O15" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="M16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="22" t="s">
+      <c r="N16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="O16" s="23" t="s">
+      <c r="O16" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="N17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="O17" s="14" t="s">
+      <c r="B17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O17" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="K18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="L18" s="16" t="s">
+      <c r="L18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M18" s="16" t="s">
+      <c r="M18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="N18" s="16" t="s">
+      <c r="N18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="17" t="s">
+      <c r="O18" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K19" s="16" t="s">
+      <c r="K19" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="L19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="M19" s="16" t="s">
+      <c r="M19" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="N19" s="16" t="s">
+      <c r="N19" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="O19" s="17" t="s">
+      <c r="O19" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="L20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="M20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="N20" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="O20" s="20" t="s">
+      <c r="B20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="22" t="s">
+      <c r="H21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="I21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="22" t="s">
+      <c r="J21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="K21" s="22" t="s">
+      <c r="K21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="22" t="s">
+      <c r="L21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M21" s="22" t="s">
+      <c r="M21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N21" s="22" t="s">
+      <c r="N21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="O21" s="23" t="s">
+      <c r="O21" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
+      <c r="B23" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7318266E-9629-B948-8A36-3C2A8EE62AC6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>